<commit_message>
upravy datového modelu, nastrel blogovy clanek
</commit_message>
<xml_diff>
--- a/Pdf_scraping_python/Licencni_prijmy/datalicence_2.xlsx
+++ b/Pdf_scraping_python/Licencni_prijmy/datalicence_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beata\OneDrive\Dokumenty\IT\Digitální akademie Czechitas\Projekt_DA_patenty\Patenty_BI\Pdf_scraping_python\Licencni_prijmy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C38545-65EB-4A6A-B4DF-87F95C67DCF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{977491F4-EEF2-4B54-84D2-90583F0D24FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="prehled" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
     <pivotCache cacheId="7" r:id="rId6"/>
     <pivotCache cacheId="12" r:id="rId7"/>
   </pivotCaches>
@@ -1539,6 +1539,8 @@
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1548,24 +1550,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -1577,6 +1567,16 @@
       <fill>
         <patternFill patternType="solid">
           <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1715,7 +1715,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Beata Motyková" refreshedDate="45619.560391898151" refreshedVersion="8" recordCount="250" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Beata Motyková" refreshedDate="45624.648290509256" refreshedVersion="8" recordCount="250" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:E251" sheet="data_licencni_prijmy"/>
   </cacheSource>
@@ -1783,7 +1783,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Beata Motyková" refreshedDate="45619.560391898151" refreshedVersion="8" recordCount="240" xr:uid="{00000000-000A-0000-FFFF-FFFF01000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Beata Motyková" refreshedDate="45624.648290740741" refreshedVersion="8" recordCount="240" xr:uid="{00000000-000A-0000-FFFF-FFFF01000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:E241" sheet="data_licencni_prijmy"/>
   </cacheSource>
@@ -5291,6 +5291,190 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="prehled 2" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="" updatedVersion="8" compact="0" compactData="0">
+  <location ref="P3:AA29" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="5">
+    <pivotField name="Nazev podsloĹľky" axis="axisRow" dataField="1" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending">
+      <items count="26">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item m="1" x="24"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField name="Nazev souboru" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0"/>
+    <pivotField name="Matching Line" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0"/>
+    <pivotField name="CASTKA" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0"/>
+    <pivotField name="ROK" axis="axisCol" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending">
+      <items count="12">
+        <item m="1" x="10"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="25">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="24"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="4"/>
+  </colFields>
+  <colItems count="11">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="COUNTA of Nazev podsloĹľky" fld="0" subtotal="count" baseField="0"/>
+  </dataFields>
+  <pivotTableStyleInfo showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000001000000}" name="prehled" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="" updatedVersion="8" compact="0" compactData="0">
   <location ref="A3:L30" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
@@ -5477,192 +5661,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="prehled 2" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="" updatedVersion="8" compact="0" compactData="0">
-  <location ref="P3:AA29" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="5">
-    <pivotField name="Nazev podsloĹľky" axis="axisRow" dataField="1" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending">
-      <items count="26">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item m="1" x="24"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="19"/>
-        <item x="20"/>
-        <item x="21"/>
-        <item x="22"/>
-        <item x="23"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField name="Nazev souboru" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0"/>
-    <pivotField name="Matching Line" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0"/>
-    <pivotField name="CASTKA" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0"/>
-    <pivotField name="ROK" axis="axisCol" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending">
-      <items count="12">
-        <item m="1" x="10"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="25">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="20"/>
-    </i>
-    <i>
-      <x v="21"/>
-    </i>
-    <i>
-      <x v="22"/>
-    </i>
-    <i>
-      <x v="23"/>
-    </i>
-    <i>
-      <x v="24"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="4"/>
-  </colFields>
-  <colItems count="11">
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="COUNTA of Nazev podsloĹľky" fld="0" subtotal="count" baseField="0"/>
-  </dataFields>
-  <pivotTableStyleInfo showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7B932626-3438-4BDA-B18E-32EA7748F8A3}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7B932626-3438-4BDA-B18E-32EA7748F8A3}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:L31" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
@@ -5839,7 +5839,7 @@
     <dataField name="Sum of CASTKA" fld="2" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="2">
-    <format dxfId="2">
+    <format dxfId="1">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1">
@@ -5853,7 +5853,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="0">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1">
@@ -6282,73 +6282,73 @@
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="16">
-        <v>1</v>
-      </c>
-      <c r="C5" s="17">
-        <v>1</v>
-      </c>
-      <c r="D5" s="17">
-        <v>1</v>
-      </c>
-      <c r="E5" s="17">
-        <v>1</v>
-      </c>
-      <c r="F5" s="17">
-        <v>1</v>
-      </c>
-      <c r="G5" s="17">
-        <v>1</v>
-      </c>
-      <c r="H5" s="17">
-        <v>1</v>
-      </c>
-      <c r="I5" s="17">
-        <v>1</v>
-      </c>
-      <c r="J5" s="17">
-        <v>1</v>
-      </c>
-      <c r="K5" s="17">
-        <v>1</v>
-      </c>
-      <c r="L5" s="18">
+      <c r="B5" s="18">
+        <v>1</v>
+      </c>
+      <c r="C5" s="19">
+        <v>1</v>
+      </c>
+      <c r="D5" s="19">
+        <v>1</v>
+      </c>
+      <c r="E5" s="19">
+        <v>1</v>
+      </c>
+      <c r="F5" s="19">
+        <v>1</v>
+      </c>
+      <c r="G5" s="19">
+        <v>1</v>
+      </c>
+      <c r="H5" s="19">
+        <v>1</v>
+      </c>
+      <c r="I5" s="19">
+        <v>1</v>
+      </c>
+      <c r="J5" s="19">
+        <v>1</v>
+      </c>
+      <c r="K5" s="19">
+        <v>1</v>
+      </c>
+      <c r="L5" s="20">
         <v>10</v>
       </c>
       <c r="P5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="Q5" s="16">
-        <v>1</v>
-      </c>
-      <c r="R5" s="17">
-        <v>1</v>
-      </c>
-      <c r="S5" s="17">
-        <v>1</v>
-      </c>
-      <c r="T5" s="17">
-        <v>1</v>
-      </c>
-      <c r="U5" s="17">
-        <v>1</v>
-      </c>
-      <c r="V5" s="17">
-        <v>1</v>
-      </c>
-      <c r="W5" s="17">
-        <v>1</v>
-      </c>
-      <c r="X5" s="17">
-        <v>1</v>
-      </c>
-      <c r="Y5" s="17">
-        <v>1</v>
-      </c>
-      <c r="Z5" s="17">
-        <v>1</v>
-      </c>
-      <c r="AA5" s="18">
+      <c r="Q5" s="18">
+        <v>1</v>
+      </c>
+      <c r="R5" s="19">
+        <v>1</v>
+      </c>
+      <c r="S5" s="19">
+        <v>1</v>
+      </c>
+      <c r="T5" s="19">
+        <v>1</v>
+      </c>
+      <c r="U5" s="19">
+        <v>1</v>
+      </c>
+      <c r="V5" s="19">
+        <v>1</v>
+      </c>
+      <c r="W5" s="19">
+        <v>1</v>
+      </c>
+      <c r="X5" s="19">
+        <v>1</v>
+      </c>
+      <c r="Y5" s="19">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="19">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="20">
         <v>10</v>
       </c>
     </row>
@@ -6356,73 +6356,73 @@
       <c r="A6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="19">
-        <v>1</v>
-      </c>
-      <c r="C6" s="20">
-        <v>1</v>
-      </c>
-      <c r="D6" s="20">
-        <v>1</v>
-      </c>
-      <c r="E6" s="20">
-        <v>1</v>
-      </c>
-      <c r="F6" s="20">
-        <v>1</v>
-      </c>
-      <c r="G6" s="20">
-        <v>1</v>
-      </c>
-      <c r="H6" s="20">
-        <v>1</v>
-      </c>
-      <c r="I6" s="20">
-        <v>1</v>
-      </c>
-      <c r="J6" s="20">
-        <v>1</v>
-      </c>
-      <c r="K6" s="20">
-        <v>1</v>
-      </c>
-      <c r="L6" s="21">
+      <c r="B6" s="21">
+        <v>1</v>
+      </c>
+      <c r="C6" s="22">
+        <v>1</v>
+      </c>
+      <c r="D6" s="22">
+        <v>1</v>
+      </c>
+      <c r="E6" s="22">
+        <v>1</v>
+      </c>
+      <c r="F6" s="22">
+        <v>1</v>
+      </c>
+      <c r="G6" s="22">
+        <v>1</v>
+      </c>
+      <c r="H6" s="22">
+        <v>1</v>
+      </c>
+      <c r="I6" s="22">
+        <v>1</v>
+      </c>
+      <c r="J6" s="22">
+        <v>1</v>
+      </c>
+      <c r="K6" s="22">
+        <v>1</v>
+      </c>
+      <c r="L6" s="23">
         <v>10</v>
       </c>
       <c r="P6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="Q6" s="19">
-        <v>1</v>
-      </c>
-      <c r="R6" s="20">
-        <v>1</v>
-      </c>
-      <c r="S6" s="20">
-        <v>1</v>
-      </c>
-      <c r="T6" s="20">
-        <v>1</v>
-      </c>
-      <c r="U6" s="20">
-        <v>1</v>
-      </c>
-      <c r="V6" s="20">
-        <v>1</v>
-      </c>
-      <c r="W6" s="20">
-        <v>1</v>
-      </c>
-      <c r="X6" s="20">
-        <v>1</v>
-      </c>
-      <c r="Y6" s="20">
-        <v>1</v>
-      </c>
-      <c r="Z6" s="20">
-        <v>1</v>
-      </c>
-      <c r="AA6" s="21">
+      <c r="Q6" s="21">
+        <v>1</v>
+      </c>
+      <c r="R6" s="22">
+        <v>1</v>
+      </c>
+      <c r="S6" s="22">
+        <v>1</v>
+      </c>
+      <c r="T6" s="22">
+        <v>1</v>
+      </c>
+      <c r="U6" s="22">
+        <v>1</v>
+      </c>
+      <c r="V6" s="22">
+        <v>1</v>
+      </c>
+      <c r="W6" s="22">
+        <v>1</v>
+      </c>
+      <c r="X6" s="22">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="22">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="22">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="23">
         <v>10</v>
       </c>
     </row>
@@ -6430,73 +6430,73 @@
       <c r="A7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="19">
-        <v>1</v>
-      </c>
-      <c r="C7" s="20">
-        <v>1</v>
-      </c>
-      <c r="D7" s="20">
-        <v>1</v>
-      </c>
-      <c r="E7" s="20">
-        <v>1</v>
-      </c>
-      <c r="F7" s="20">
-        <v>1</v>
-      </c>
-      <c r="G7" s="20">
-        <v>1</v>
-      </c>
-      <c r="H7" s="20">
-        <v>1</v>
-      </c>
-      <c r="I7" s="20">
-        <v>1</v>
-      </c>
-      <c r="J7" s="20">
-        <v>1</v>
-      </c>
-      <c r="K7" s="20">
-        <v>1</v>
-      </c>
-      <c r="L7" s="21">
+      <c r="B7" s="21">
+        <v>1</v>
+      </c>
+      <c r="C7" s="22">
+        <v>1</v>
+      </c>
+      <c r="D7" s="22">
+        <v>1</v>
+      </c>
+      <c r="E7" s="22">
+        <v>1</v>
+      </c>
+      <c r="F7" s="22">
+        <v>1</v>
+      </c>
+      <c r="G7" s="22">
+        <v>1</v>
+      </c>
+      <c r="H7" s="22">
+        <v>1</v>
+      </c>
+      <c r="I7" s="22">
+        <v>1</v>
+      </c>
+      <c r="J7" s="22">
+        <v>1</v>
+      </c>
+      <c r="K7" s="22">
+        <v>1</v>
+      </c>
+      <c r="L7" s="23">
         <v>10</v>
       </c>
       <c r="P7" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="Q7" s="19">
-        <v>1</v>
-      </c>
-      <c r="R7" s="20">
-        <v>1</v>
-      </c>
-      <c r="S7" s="20">
-        <v>1</v>
-      </c>
-      <c r="T7" s="20">
-        <v>1</v>
-      </c>
-      <c r="U7" s="20">
-        <v>1</v>
-      </c>
-      <c r="V7" s="20">
-        <v>1</v>
-      </c>
-      <c r="W7" s="20">
-        <v>1</v>
-      </c>
-      <c r="X7" s="20">
-        <v>1</v>
-      </c>
-      <c r="Y7" s="20">
-        <v>1</v>
-      </c>
-      <c r="Z7" s="20">
-        <v>1</v>
-      </c>
-      <c r="AA7" s="21">
+      <c r="Q7" s="21">
+        <v>1</v>
+      </c>
+      <c r="R7" s="22">
+        <v>1</v>
+      </c>
+      <c r="S7" s="22">
+        <v>1</v>
+      </c>
+      <c r="T7" s="22">
+        <v>1</v>
+      </c>
+      <c r="U7" s="22">
+        <v>1</v>
+      </c>
+      <c r="V7" s="22">
+        <v>1</v>
+      </c>
+      <c r="W7" s="22">
+        <v>1</v>
+      </c>
+      <c r="X7" s="22">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="22">
+        <v>1</v>
+      </c>
+      <c r="Z7" s="22">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="23">
         <v>10</v>
       </c>
     </row>
@@ -6504,73 +6504,73 @@
       <c r="A8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="19">
-        <v>1</v>
-      </c>
-      <c r="C8" s="20">
-        <v>1</v>
-      </c>
-      <c r="D8" s="20">
-        <v>1</v>
-      </c>
-      <c r="E8" s="20">
-        <v>1</v>
-      </c>
-      <c r="F8" s="20">
-        <v>1</v>
-      </c>
-      <c r="G8" s="20">
-        <v>1</v>
-      </c>
-      <c r="H8" s="20">
-        <v>1</v>
-      </c>
-      <c r="I8" s="20">
-        <v>1</v>
-      </c>
-      <c r="J8" s="20">
-        <v>1</v>
-      </c>
-      <c r="K8" s="20">
-        <v>1</v>
-      </c>
-      <c r="L8" s="21">
+      <c r="B8" s="21">
+        <v>1</v>
+      </c>
+      <c r="C8" s="22">
+        <v>1</v>
+      </c>
+      <c r="D8" s="22">
+        <v>1</v>
+      </c>
+      <c r="E8" s="22">
+        <v>1</v>
+      </c>
+      <c r="F8" s="22">
+        <v>1</v>
+      </c>
+      <c r="G8" s="22">
+        <v>1</v>
+      </c>
+      <c r="H8" s="22">
+        <v>1</v>
+      </c>
+      <c r="I8" s="22">
+        <v>1</v>
+      </c>
+      <c r="J8" s="22">
+        <v>1</v>
+      </c>
+      <c r="K8" s="22">
+        <v>1</v>
+      </c>
+      <c r="L8" s="23">
         <v>10</v>
       </c>
       <c r="P8" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="Q8" s="19">
-        <v>1</v>
-      </c>
-      <c r="R8" s="20">
-        <v>1</v>
-      </c>
-      <c r="S8" s="20">
-        <v>1</v>
-      </c>
-      <c r="T8" s="20">
-        <v>1</v>
-      </c>
-      <c r="U8" s="20">
-        <v>1</v>
-      </c>
-      <c r="V8" s="20">
-        <v>1</v>
-      </c>
-      <c r="W8" s="20">
-        <v>1</v>
-      </c>
-      <c r="X8" s="20">
-        <v>1</v>
-      </c>
-      <c r="Y8" s="20">
-        <v>1</v>
-      </c>
-      <c r="Z8" s="20">
-        <v>1</v>
-      </c>
-      <c r="AA8" s="21">
+      <c r="Q8" s="21">
+        <v>1</v>
+      </c>
+      <c r="R8" s="22">
+        <v>1</v>
+      </c>
+      <c r="S8" s="22">
+        <v>1</v>
+      </c>
+      <c r="T8" s="22">
+        <v>1</v>
+      </c>
+      <c r="U8" s="22">
+        <v>1</v>
+      </c>
+      <c r="V8" s="22">
+        <v>1</v>
+      </c>
+      <c r="W8" s="22">
+        <v>1</v>
+      </c>
+      <c r="X8" s="22">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="22">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="22">
+        <v>1</v>
+      </c>
+      <c r="AA8" s="23">
         <v>10</v>
       </c>
     </row>
@@ -6578,73 +6578,73 @@
       <c r="A9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="19">
-        <v>1</v>
-      </c>
-      <c r="C9" s="20">
-        <v>1</v>
-      </c>
-      <c r="D9" s="20">
-        <v>1</v>
-      </c>
-      <c r="E9" s="20">
-        <v>1</v>
-      </c>
-      <c r="F9" s="20">
-        <v>1</v>
-      </c>
-      <c r="G9" s="20">
-        <v>1</v>
-      </c>
-      <c r="H9" s="20">
-        <v>1</v>
-      </c>
-      <c r="I9" s="20">
-        <v>1</v>
-      </c>
-      <c r="J9" s="20">
-        <v>1</v>
-      </c>
-      <c r="K9" s="20">
-        <v>1</v>
-      </c>
-      <c r="L9" s="21">
+      <c r="B9" s="21">
+        <v>1</v>
+      </c>
+      <c r="C9" s="22">
+        <v>1</v>
+      </c>
+      <c r="D9" s="22">
+        <v>1</v>
+      </c>
+      <c r="E9" s="22">
+        <v>1</v>
+      </c>
+      <c r="F9" s="22">
+        <v>1</v>
+      </c>
+      <c r="G9" s="22">
+        <v>1</v>
+      </c>
+      <c r="H9" s="22">
+        <v>1</v>
+      </c>
+      <c r="I9" s="22">
+        <v>1</v>
+      </c>
+      <c r="J9" s="22">
+        <v>1</v>
+      </c>
+      <c r="K9" s="22">
+        <v>1</v>
+      </c>
+      <c r="L9" s="23">
         <v>10</v>
       </c>
       <c r="P9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="Q9" s="19">
-        <v>1</v>
-      </c>
-      <c r="R9" s="20">
-        <v>1</v>
-      </c>
-      <c r="S9" s="20">
-        <v>1</v>
-      </c>
-      <c r="T9" s="20">
-        <v>1</v>
-      </c>
-      <c r="U9" s="20">
-        <v>1</v>
-      </c>
-      <c r="V9" s="20">
-        <v>1</v>
-      </c>
-      <c r="W9" s="20">
-        <v>1</v>
-      </c>
-      <c r="X9" s="20">
-        <v>1</v>
-      </c>
-      <c r="Y9" s="20">
-        <v>1</v>
-      </c>
-      <c r="Z9" s="20">
-        <v>1</v>
-      </c>
-      <c r="AA9" s="21">
+      <c r="Q9" s="21">
+        <v>1</v>
+      </c>
+      <c r="R9" s="22">
+        <v>1</v>
+      </c>
+      <c r="S9" s="22">
+        <v>1</v>
+      </c>
+      <c r="T9" s="22">
+        <v>1</v>
+      </c>
+      <c r="U9" s="22">
+        <v>1</v>
+      </c>
+      <c r="V9" s="22">
+        <v>1</v>
+      </c>
+      <c r="W9" s="22">
+        <v>1</v>
+      </c>
+      <c r="X9" s="22">
+        <v>1</v>
+      </c>
+      <c r="Y9" s="22">
+        <v>1</v>
+      </c>
+      <c r="Z9" s="22">
+        <v>1</v>
+      </c>
+      <c r="AA9" s="23">
         <v>10</v>
       </c>
     </row>
@@ -6652,73 +6652,73 @@
       <c r="A10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="19">
-        <v>1</v>
-      </c>
-      <c r="C10" s="20">
-        <v>1</v>
-      </c>
-      <c r="D10" s="20">
-        <v>1</v>
-      </c>
-      <c r="E10" s="20">
-        <v>1</v>
-      </c>
-      <c r="F10" s="20">
-        <v>1</v>
-      </c>
-      <c r="G10" s="20">
-        <v>1</v>
-      </c>
-      <c r="H10" s="20">
-        <v>1</v>
-      </c>
-      <c r="I10" s="20">
-        <v>1</v>
-      </c>
-      <c r="J10" s="20">
-        <v>1</v>
-      </c>
-      <c r="K10" s="20">
-        <v>1</v>
-      </c>
-      <c r="L10" s="21">
+      <c r="B10" s="21">
+        <v>1</v>
+      </c>
+      <c r="C10" s="22">
+        <v>1</v>
+      </c>
+      <c r="D10" s="22">
+        <v>1</v>
+      </c>
+      <c r="E10" s="22">
+        <v>1</v>
+      </c>
+      <c r="F10" s="22">
+        <v>1</v>
+      </c>
+      <c r="G10" s="22">
+        <v>1</v>
+      </c>
+      <c r="H10" s="22">
+        <v>1</v>
+      </c>
+      <c r="I10" s="22">
+        <v>1</v>
+      </c>
+      <c r="J10" s="22">
+        <v>1</v>
+      </c>
+      <c r="K10" s="22">
+        <v>1</v>
+      </c>
+      <c r="L10" s="23">
         <v>10</v>
       </c>
       <c r="P10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="Q10" s="19">
-        <v>1</v>
-      </c>
-      <c r="R10" s="20">
-        <v>1</v>
-      </c>
-      <c r="S10" s="20">
-        <v>1</v>
-      </c>
-      <c r="T10" s="20">
-        <v>1</v>
-      </c>
-      <c r="U10" s="20">
-        <v>1</v>
-      </c>
-      <c r="V10" s="20">
-        <v>1</v>
-      </c>
-      <c r="W10" s="20">
-        <v>1</v>
-      </c>
-      <c r="X10" s="20">
-        <v>1</v>
-      </c>
-      <c r="Y10" s="20">
-        <v>1</v>
-      </c>
-      <c r="Z10" s="20">
-        <v>1</v>
-      </c>
-      <c r="AA10" s="21">
+      <c r="Q10" s="21">
+        <v>1</v>
+      </c>
+      <c r="R10" s="22">
+        <v>1</v>
+      </c>
+      <c r="S10" s="22">
+        <v>1</v>
+      </c>
+      <c r="T10" s="22">
+        <v>1</v>
+      </c>
+      <c r="U10" s="22">
+        <v>1</v>
+      </c>
+      <c r="V10" s="22">
+        <v>1</v>
+      </c>
+      <c r="W10" s="22">
+        <v>1</v>
+      </c>
+      <c r="X10" s="22">
+        <v>1</v>
+      </c>
+      <c r="Y10" s="22">
+        <v>1</v>
+      </c>
+      <c r="Z10" s="22">
+        <v>1</v>
+      </c>
+      <c r="AA10" s="23">
         <v>10</v>
       </c>
     </row>
@@ -6726,73 +6726,73 @@
       <c r="A11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="19">
-        <v>1</v>
-      </c>
-      <c r="C11" s="20">
-        <v>1</v>
-      </c>
-      <c r="D11" s="20">
-        <v>1</v>
-      </c>
-      <c r="E11" s="20">
-        <v>1</v>
-      </c>
-      <c r="F11" s="20">
-        <v>1</v>
-      </c>
-      <c r="G11" s="20">
-        <v>1</v>
-      </c>
-      <c r="H11" s="20">
-        <v>1</v>
-      </c>
-      <c r="I11" s="20">
-        <v>1</v>
-      </c>
-      <c r="J11" s="20">
-        <v>1</v>
-      </c>
-      <c r="K11" s="20">
-        <v>1</v>
-      </c>
-      <c r="L11" s="21">
+      <c r="B11" s="21">
+        <v>1</v>
+      </c>
+      <c r="C11" s="22">
+        <v>1</v>
+      </c>
+      <c r="D11" s="22">
+        <v>1</v>
+      </c>
+      <c r="E11" s="22">
+        <v>1</v>
+      </c>
+      <c r="F11" s="22">
+        <v>1</v>
+      </c>
+      <c r="G11" s="22">
+        <v>1</v>
+      </c>
+      <c r="H11" s="22">
+        <v>1</v>
+      </c>
+      <c r="I11" s="22">
+        <v>1</v>
+      </c>
+      <c r="J11" s="22">
+        <v>1</v>
+      </c>
+      <c r="K11" s="22">
+        <v>1</v>
+      </c>
+      <c r="L11" s="23">
         <v>10</v>
       </c>
       <c r="P11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="Q11" s="19">
-        <v>1</v>
-      </c>
-      <c r="R11" s="20">
-        <v>1</v>
-      </c>
-      <c r="S11" s="20">
-        <v>1</v>
-      </c>
-      <c r="T11" s="20">
-        <v>1</v>
-      </c>
-      <c r="U11" s="20">
-        <v>1</v>
-      </c>
-      <c r="V11" s="20">
-        <v>1</v>
-      </c>
-      <c r="W11" s="20">
-        <v>1</v>
-      </c>
-      <c r="X11" s="20">
-        <v>1</v>
-      </c>
-      <c r="Y11" s="20">
-        <v>1</v>
-      </c>
-      <c r="Z11" s="20">
-        <v>1</v>
-      </c>
-      <c r="AA11" s="21">
+      <c r="Q11" s="21">
+        <v>1</v>
+      </c>
+      <c r="R11" s="22">
+        <v>1</v>
+      </c>
+      <c r="S11" s="22">
+        <v>1</v>
+      </c>
+      <c r="T11" s="22">
+        <v>1</v>
+      </c>
+      <c r="U11" s="22">
+        <v>1</v>
+      </c>
+      <c r="V11" s="22">
+        <v>1</v>
+      </c>
+      <c r="W11" s="22">
+        <v>1</v>
+      </c>
+      <c r="X11" s="22">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="22">
+        <v>1</v>
+      </c>
+      <c r="Z11" s="22">
+        <v>1</v>
+      </c>
+      <c r="AA11" s="23">
         <v>10</v>
       </c>
     </row>
@@ -6800,73 +6800,73 @@
       <c r="A12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="19">
-        <v>1</v>
-      </c>
-      <c r="C12" s="20">
-        <v>1</v>
-      </c>
-      <c r="D12" s="20">
-        <v>1</v>
-      </c>
-      <c r="E12" s="20">
-        <v>1</v>
-      </c>
-      <c r="F12" s="20">
-        <v>1</v>
-      </c>
-      <c r="G12" s="20">
-        <v>1</v>
-      </c>
-      <c r="H12" s="20">
-        <v>1</v>
-      </c>
-      <c r="I12" s="20">
-        <v>1</v>
-      </c>
-      <c r="J12" s="20">
-        <v>1</v>
-      </c>
-      <c r="K12" s="20">
-        <v>1</v>
-      </c>
-      <c r="L12" s="21">
+      <c r="B12" s="21">
+        <v>1</v>
+      </c>
+      <c r="C12" s="22">
+        <v>1</v>
+      </c>
+      <c r="D12" s="22">
+        <v>1</v>
+      </c>
+      <c r="E12" s="22">
+        <v>1</v>
+      </c>
+      <c r="F12" s="22">
+        <v>1</v>
+      </c>
+      <c r="G12" s="22">
+        <v>1</v>
+      </c>
+      <c r="H12" s="22">
+        <v>1</v>
+      </c>
+      <c r="I12" s="22">
+        <v>1</v>
+      </c>
+      <c r="J12" s="22">
+        <v>1</v>
+      </c>
+      <c r="K12" s="22">
+        <v>1</v>
+      </c>
+      <c r="L12" s="23">
         <v>10</v>
       </c>
       <c r="P12" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="Q12" s="19">
-        <v>1</v>
-      </c>
-      <c r="R12" s="20">
-        <v>1</v>
-      </c>
-      <c r="S12" s="20">
-        <v>1</v>
-      </c>
-      <c r="T12" s="20">
-        <v>1</v>
-      </c>
-      <c r="U12" s="20">
-        <v>1</v>
-      </c>
-      <c r="V12" s="20">
-        <v>1</v>
-      </c>
-      <c r="W12" s="20">
-        <v>1</v>
-      </c>
-      <c r="X12" s="20">
-        <v>1</v>
-      </c>
-      <c r="Y12" s="20">
-        <v>1</v>
-      </c>
-      <c r="Z12" s="20">
-        <v>1</v>
-      </c>
-      <c r="AA12" s="21">
+      <c r="Q12" s="21">
+        <v>1</v>
+      </c>
+      <c r="R12" s="22">
+        <v>1</v>
+      </c>
+      <c r="S12" s="22">
+        <v>1</v>
+      </c>
+      <c r="T12" s="22">
+        <v>1</v>
+      </c>
+      <c r="U12" s="22">
+        <v>1</v>
+      </c>
+      <c r="V12" s="22">
+        <v>1</v>
+      </c>
+      <c r="W12" s="22">
+        <v>1</v>
+      </c>
+      <c r="X12" s="22">
+        <v>1</v>
+      </c>
+      <c r="Y12" s="22">
+        <v>1</v>
+      </c>
+      <c r="Z12" s="22">
+        <v>1</v>
+      </c>
+      <c r="AA12" s="23">
         <v>10</v>
       </c>
     </row>
@@ -6874,73 +6874,73 @@
       <c r="A13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="19">
-        <v>1</v>
-      </c>
-      <c r="C13" s="20">
-        <v>1</v>
-      </c>
-      <c r="D13" s="20">
-        <v>1</v>
-      </c>
-      <c r="E13" s="20">
-        <v>1</v>
-      </c>
-      <c r="F13" s="20">
-        <v>1</v>
-      </c>
-      <c r="G13" s="20">
-        <v>1</v>
-      </c>
-      <c r="H13" s="20">
-        <v>1</v>
-      </c>
-      <c r="I13" s="20">
-        <v>1</v>
-      </c>
-      <c r="J13" s="20">
-        <v>1</v>
-      </c>
-      <c r="K13" s="20">
-        <v>1</v>
-      </c>
-      <c r="L13" s="21">
+      <c r="B13" s="21">
+        <v>1</v>
+      </c>
+      <c r="C13" s="22">
+        <v>1</v>
+      </c>
+      <c r="D13" s="22">
+        <v>1</v>
+      </c>
+      <c r="E13" s="22">
+        <v>1</v>
+      </c>
+      <c r="F13" s="22">
+        <v>1</v>
+      </c>
+      <c r="G13" s="22">
+        <v>1</v>
+      </c>
+      <c r="H13" s="22">
+        <v>1</v>
+      </c>
+      <c r="I13" s="22">
+        <v>1</v>
+      </c>
+      <c r="J13" s="22">
+        <v>1</v>
+      </c>
+      <c r="K13" s="22">
+        <v>1</v>
+      </c>
+      <c r="L13" s="23">
         <v>10</v>
       </c>
       <c r="P13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="Q13" s="19">
-        <v>1</v>
-      </c>
-      <c r="R13" s="20">
-        <v>1</v>
-      </c>
-      <c r="S13" s="20">
-        <v>1</v>
-      </c>
-      <c r="T13" s="20">
-        <v>1</v>
-      </c>
-      <c r="U13" s="20">
-        <v>1</v>
-      </c>
-      <c r="V13" s="20">
-        <v>1</v>
-      </c>
-      <c r="W13" s="20">
-        <v>1</v>
-      </c>
-      <c r="X13" s="20">
-        <v>1</v>
-      </c>
-      <c r="Y13" s="20">
-        <v>1</v>
-      </c>
-      <c r="Z13" s="20">
-        <v>1</v>
-      </c>
-      <c r="AA13" s="21">
+      <c r="Q13" s="21">
+        <v>1</v>
+      </c>
+      <c r="R13" s="22">
+        <v>1</v>
+      </c>
+      <c r="S13" s="22">
+        <v>1</v>
+      </c>
+      <c r="T13" s="22">
+        <v>1</v>
+      </c>
+      <c r="U13" s="22">
+        <v>1</v>
+      </c>
+      <c r="V13" s="22">
+        <v>1</v>
+      </c>
+      <c r="W13" s="22">
+        <v>1</v>
+      </c>
+      <c r="X13" s="22">
+        <v>1</v>
+      </c>
+      <c r="Y13" s="22">
+        <v>1</v>
+      </c>
+      <c r="Z13" s="22">
+        <v>1</v>
+      </c>
+      <c r="AA13" s="23">
         <v>10</v>
       </c>
     </row>
@@ -6948,73 +6948,73 @@
       <c r="A14" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="19">
-        <v>1</v>
-      </c>
-      <c r="C14" s="20">
-        <v>1</v>
-      </c>
-      <c r="D14" s="20">
-        <v>1</v>
-      </c>
-      <c r="E14" s="20">
-        <v>1</v>
-      </c>
-      <c r="F14" s="20">
-        <v>1</v>
-      </c>
-      <c r="G14" s="20">
-        <v>1</v>
-      </c>
-      <c r="H14" s="20">
-        <v>1</v>
-      </c>
-      <c r="I14" s="20">
-        <v>1</v>
-      </c>
-      <c r="J14" s="20">
-        <v>1</v>
-      </c>
-      <c r="K14" s="20">
-        <v>1</v>
-      </c>
-      <c r="L14" s="21">
+      <c r="B14" s="21">
+        <v>1</v>
+      </c>
+      <c r="C14" s="22">
+        <v>1</v>
+      </c>
+      <c r="D14" s="22">
+        <v>1</v>
+      </c>
+      <c r="E14" s="22">
+        <v>1</v>
+      </c>
+      <c r="F14" s="22">
+        <v>1</v>
+      </c>
+      <c r="G14" s="22">
+        <v>1</v>
+      </c>
+      <c r="H14" s="22">
+        <v>1</v>
+      </c>
+      <c r="I14" s="22">
+        <v>1</v>
+      </c>
+      <c r="J14" s="22">
+        <v>1</v>
+      </c>
+      <c r="K14" s="22">
+        <v>1</v>
+      </c>
+      <c r="L14" s="23">
         <v>10</v>
       </c>
       <c r="P14" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="Q14" s="19">
-        <v>1</v>
-      </c>
-      <c r="R14" s="20">
-        <v>1</v>
-      </c>
-      <c r="S14" s="20">
-        <v>1</v>
-      </c>
-      <c r="T14" s="20">
-        <v>1</v>
-      </c>
-      <c r="U14" s="20">
-        <v>1</v>
-      </c>
-      <c r="V14" s="20">
-        <v>1</v>
-      </c>
-      <c r="W14" s="20">
-        <v>1</v>
-      </c>
-      <c r="X14" s="20">
-        <v>1</v>
-      </c>
-      <c r="Y14" s="20">
-        <v>1</v>
-      </c>
-      <c r="Z14" s="20">
-        <v>1</v>
-      </c>
-      <c r="AA14" s="21">
+      <c r="Q14" s="21">
+        <v>1</v>
+      </c>
+      <c r="R14" s="22">
+        <v>1</v>
+      </c>
+      <c r="S14" s="22">
+        <v>1</v>
+      </c>
+      <c r="T14" s="22">
+        <v>1</v>
+      </c>
+      <c r="U14" s="22">
+        <v>1</v>
+      </c>
+      <c r="V14" s="22">
+        <v>1</v>
+      </c>
+      <c r="W14" s="22">
+        <v>1</v>
+      </c>
+      <c r="X14" s="22">
+        <v>1</v>
+      </c>
+      <c r="Y14" s="22">
+        <v>1</v>
+      </c>
+      <c r="Z14" s="22">
+        <v>1</v>
+      </c>
+      <c r="AA14" s="23">
         <v>10</v>
       </c>
     </row>
@@ -7022,73 +7022,73 @@
       <c r="A15" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="19">
-        <v>1</v>
-      </c>
-      <c r="C15" s="20">
-        <v>1</v>
-      </c>
-      <c r="D15" s="20">
-        <v>1</v>
-      </c>
-      <c r="E15" s="20">
-        <v>1</v>
-      </c>
-      <c r="F15" s="20">
-        <v>1</v>
-      </c>
-      <c r="G15" s="20">
-        <v>1</v>
-      </c>
-      <c r="H15" s="20">
-        <v>1</v>
-      </c>
-      <c r="I15" s="20">
-        <v>1</v>
-      </c>
-      <c r="J15" s="20">
-        <v>1</v>
-      </c>
-      <c r="K15" s="20">
-        <v>1</v>
-      </c>
-      <c r="L15" s="21">
+      <c r="B15" s="21">
+        <v>1</v>
+      </c>
+      <c r="C15" s="22">
+        <v>1</v>
+      </c>
+      <c r="D15" s="22">
+        <v>1</v>
+      </c>
+      <c r="E15" s="22">
+        <v>1</v>
+      </c>
+      <c r="F15" s="22">
+        <v>1</v>
+      </c>
+      <c r="G15" s="22">
+        <v>1</v>
+      </c>
+      <c r="H15" s="22">
+        <v>1</v>
+      </c>
+      <c r="I15" s="22">
+        <v>1</v>
+      </c>
+      <c r="J15" s="22">
+        <v>1</v>
+      </c>
+      <c r="K15" s="22">
+        <v>1</v>
+      </c>
+      <c r="L15" s="23">
         <v>10</v>
       </c>
       <c r="P15" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="Q15" s="19">
-        <v>1</v>
-      </c>
-      <c r="R15" s="20">
-        <v>1</v>
-      </c>
-      <c r="S15" s="20">
-        <v>1</v>
-      </c>
-      <c r="T15" s="20">
-        <v>1</v>
-      </c>
-      <c r="U15" s="20">
-        <v>1</v>
-      </c>
-      <c r="V15" s="20">
-        <v>1</v>
-      </c>
-      <c r="W15" s="20">
-        <v>1</v>
-      </c>
-      <c r="X15" s="20">
-        <v>1</v>
-      </c>
-      <c r="Y15" s="20">
-        <v>1</v>
-      </c>
-      <c r="Z15" s="20">
-        <v>1</v>
-      </c>
-      <c r="AA15" s="21">
+      <c r="Q15" s="21">
+        <v>1</v>
+      </c>
+      <c r="R15" s="22">
+        <v>1</v>
+      </c>
+      <c r="S15" s="22">
+        <v>1</v>
+      </c>
+      <c r="T15" s="22">
+        <v>1</v>
+      </c>
+      <c r="U15" s="22">
+        <v>1</v>
+      </c>
+      <c r="V15" s="22">
+        <v>1</v>
+      </c>
+      <c r="W15" s="22">
+        <v>1</v>
+      </c>
+      <c r="X15" s="22">
+        <v>1</v>
+      </c>
+      <c r="Y15" s="22">
+        <v>1</v>
+      </c>
+      <c r="Z15" s="22">
+        <v>1</v>
+      </c>
+      <c r="AA15" s="23">
         <v>10</v>
       </c>
     </row>
@@ -7096,73 +7096,73 @@
       <c r="A16" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="19">
-        <v>1</v>
-      </c>
-      <c r="C16" s="20">
-        <v>1</v>
-      </c>
-      <c r="D16" s="20">
-        <v>1</v>
-      </c>
-      <c r="E16" s="20">
-        <v>1</v>
-      </c>
-      <c r="F16" s="20">
-        <v>1</v>
-      </c>
-      <c r="G16" s="20">
-        <v>1</v>
-      </c>
-      <c r="H16" s="20">
-        <v>1</v>
-      </c>
-      <c r="I16" s="20">
-        <v>1</v>
-      </c>
-      <c r="J16" s="20">
-        <v>1</v>
-      </c>
-      <c r="K16" s="20">
-        <v>1</v>
-      </c>
-      <c r="L16" s="21">
+      <c r="B16" s="21">
+        <v>1</v>
+      </c>
+      <c r="C16" s="22">
+        <v>1</v>
+      </c>
+      <c r="D16" s="22">
+        <v>1</v>
+      </c>
+      <c r="E16" s="22">
+        <v>1</v>
+      </c>
+      <c r="F16" s="22">
+        <v>1</v>
+      </c>
+      <c r="G16" s="22">
+        <v>1</v>
+      </c>
+      <c r="H16" s="22">
+        <v>1</v>
+      </c>
+      <c r="I16" s="22">
+        <v>1</v>
+      </c>
+      <c r="J16" s="22">
+        <v>1</v>
+      </c>
+      <c r="K16" s="22">
+        <v>1</v>
+      </c>
+      <c r="L16" s="23">
         <v>10</v>
       </c>
       <c r="P16" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="Q16" s="19">
-        <v>1</v>
-      </c>
-      <c r="R16" s="20">
-        <v>1</v>
-      </c>
-      <c r="S16" s="20">
-        <v>1</v>
-      </c>
-      <c r="T16" s="20">
-        <v>1</v>
-      </c>
-      <c r="U16" s="20">
-        <v>1</v>
-      </c>
-      <c r="V16" s="20">
-        <v>1</v>
-      </c>
-      <c r="W16" s="20">
-        <v>1</v>
-      </c>
-      <c r="X16" s="20">
-        <v>1</v>
-      </c>
-      <c r="Y16" s="20">
-        <v>1</v>
-      </c>
-      <c r="Z16" s="20">
-        <v>1</v>
-      </c>
-      <c r="AA16" s="21">
+      <c r="Q16" s="21">
+        <v>1</v>
+      </c>
+      <c r="R16" s="22">
+        <v>1</v>
+      </c>
+      <c r="S16" s="22">
+        <v>1</v>
+      </c>
+      <c r="T16" s="22">
+        <v>1</v>
+      </c>
+      <c r="U16" s="22">
+        <v>1</v>
+      </c>
+      <c r="V16" s="22">
+        <v>1</v>
+      </c>
+      <c r="W16" s="22">
+        <v>1</v>
+      </c>
+      <c r="X16" s="22">
+        <v>1</v>
+      </c>
+      <c r="Y16" s="22">
+        <v>1</v>
+      </c>
+      <c r="Z16" s="22">
+        <v>1</v>
+      </c>
+      <c r="AA16" s="23">
         <v>10</v>
       </c>
     </row>
@@ -7170,73 +7170,73 @@
       <c r="A17" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="19">
-        <v>1</v>
-      </c>
-      <c r="C17" s="20">
-        <v>1</v>
-      </c>
-      <c r="D17" s="20">
-        <v>1</v>
-      </c>
-      <c r="E17" s="20">
-        <v>1</v>
-      </c>
-      <c r="F17" s="20">
-        <v>1</v>
-      </c>
-      <c r="G17" s="20">
-        <v>1</v>
-      </c>
-      <c r="H17" s="20">
-        <v>1</v>
-      </c>
-      <c r="I17" s="20">
-        <v>1</v>
-      </c>
-      <c r="J17" s="20">
-        <v>1</v>
-      </c>
-      <c r="K17" s="20">
-        <v>1</v>
-      </c>
-      <c r="L17" s="21">
+      <c r="B17" s="21">
+        <v>1</v>
+      </c>
+      <c r="C17" s="22">
+        <v>1</v>
+      </c>
+      <c r="D17" s="22">
+        <v>1</v>
+      </c>
+      <c r="E17" s="22">
+        <v>1</v>
+      </c>
+      <c r="F17" s="22">
+        <v>1</v>
+      </c>
+      <c r="G17" s="22">
+        <v>1</v>
+      </c>
+      <c r="H17" s="22">
+        <v>1</v>
+      </c>
+      <c r="I17" s="22">
+        <v>1</v>
+      </c>
+      <c r="J17" s="22">
+        <v>1</v>
+      </c>
+      <c r="K17" s="22">
+        <v>1</v>
+      </c>
+      <c r="L17" s="23">
         <v>10</v>
       </c>
       <c r="P17" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="Q17" s="19">
-        <v>1</v>
-      </c>
-      <c r="R17" s="20">
-        <v>1</v>
-      </c>
-      <c r="S17" s="20">
-        <v>1</v>
-      </c>
-      <c r="T17" s="20">
-        <v>1</v>
-      </c>
-      <c r="U17" s="20">
-        <v>1</v>
-      </c>
-      <c r="V17" s="20">
-        <v>1</v>
-      </c>
-      <c r="W17" s="20">
-        <v>1</v>
-      </c>
-      <c r="X17" s="20">
-        <v>1</v>
-      </c>
-      <c r="Y17" s="20">
-        <v>1</v>
-      </c>
-      <c r="Z17" s="20">
-        <v>1</v>
-      </c>
-      <c r="AA17" s="21">
+      <c r="Q17" s="21">
+        <v>1</v>
+      </c>
+      <c r="R17" s="22">
+        <v>1</v>
+      </c>
+      <c r="S17" s="22">
+        <v>1</v>
+      </c>
+      <c r="T17" s="22">
+        <v>1</v>
+      </c>
+      <c r="U17" s="22">
+        <v>1</v>
+      </c>
+      <c r="V17" s="22">
+        <v>1</v>
+      </c>
+      <c r="W17" s="22">
+        <v>1</v>
+      </c>
+      <c r="X17" s="22">
+        <v>1</v>
+      </c>
+      <c r="Y17" s="22">
+        <v>1</v>
+      </c>
+      <c r="Z17" s="22">
+        <v>1</v>
+      </c>
+      <c r="AA17" s="23">
         <v>10</v>
       </c>
     </row>
@@ -7244,73 +7244,73 @@
       <c r="A18" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="19">
-        <v>1</v>
-      </c>
-      <c r="C18" s="20">
-        <v>1</v>
-      </c>
-      <c r="D18" s="20">
-        <v>1</v>
-      </c>
-      <c r="E18" s="20">
-        <v>1</v>
-      </c>
-      <c r="F18" s="20">
-        <v>1</v>
-      </c>
-      <c r="G18" s="20">
-        <v>1</v>
-      </c>
-      <c r="H18" s="20">
-        <v>1</v>
-      </c>
-      <c r="I18" s="20">
-        <v>1</v>
-      </c>
-      <c r="J18" s="20">
-        <v>1</v>
-      </c>
-      <c r="K18" s="20">
-        <v>1</v>
-      </c>
-      <c r="L18" s="21">
+      <c r="B18" s="21">
+        <v>1</v>
+      </c>
+      <c r="C18" s="22">
+        <v>1</v>
+      </c>
+      <c r="D18" s="22">
+        <v>1</v>
+      </c>
+      <c r="E18" s="22">
+        <v>1</v>
+      </c>
+      <c r="F18" s="22">
+        <v>1</v>
+      </c>
+      <c r="G18" s="22">
+        <v>1</v>
+      </c>
+      <c r="H18" s="22">
+        <v>1</v>
+      </c>
+      <c r="I18" s="22">
+        <v>1</v>
+      </c>
+      <c r="J18" s="22">
+        <v>1</v>
+      </c>
+      <c r="K18" s="22">
+        <v>1</v>
+      </c>
+      <c r="L18" s="23">
         <v>10</v>
       </c>
       <c r="P18" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="Q18" s="19">
-        <v>1</v>
-      </c>
-      <c r="R18" s="20">
-        <v>1</v>
-      </c>
-      <c r="S18" s="20">
-        <v>1</v>
-      </c>
-      <c r="T18" s="20">
-        <v>1</v>
-      </c>
-      <c r="U18" s="20">
-        <v>1</v>
-      </c>
-      <c r="V18" s="20">
-        <v>1</v>
-      </c>
-      <c r="W18" s="20">
-        <v>1</v>
-      </c>
-      <c r="X18" s="20">
-        <v>1</v>
-      </c>
-      <c r="Y18" s="20">
-        <v>1</v>
-      </c>
-      <c r="Z18" s="20">
-        <v>1</v>
-      </c>
-      <c r="AA18" s="21">
+      <c r="Q18" s="21">
+        <v>1</v>
+      </c>
+      <c r="R18" s="22">
+        <v>1</v>
+      </c>
+      <c r="S18" s="22">
+        <v>1</v>
+      </c>
+      <c r="T18" s="22">
+        <v>1</v>
+      </c>
+      <c r="U18" s="22">
+        <v>1</v>
+      </c>
+      <c r="V18" s="22">
+        <v>1</v>
+      </c>
+      <c r="W18" s="22">
+        <v>1</v>
+      </c>
+      <c r="X18" s="22">
+        <v>1</v>
+      </c>
+      <c r="Y18" s="22">
+        <v>1</v>
+      </c>
+      <c r="Z18" s="22">
+        <v>1</v>
+      </c>
+      <c r="AA18" s="23">
         <v>10</v>
       </c>
     </row>
@@ -7318,73 +7318,73 @@
       <c r="A19" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="19">
-        <v>1</v>
-      </c>
-      <c r="C19" s="20">
-        <v>1</v>
-      </c>
-      <c r="D19" s="20">
-        <v>1</v>
-      </c>
-      <c r="E19" s="20">
-        <v>1</v>
-      </c>
-      <c r="F19" s="20">
-        <v>1</v>
-      </c>
-      <c r="G19" s="20">
-        <v>1</v>
-      </c>
-      <c r="H19" s="20">
-        <v>1</v>
-      </c>
-      <c r="I19" s="20">
-        <v>1</v>
-      </c>
-      <c r="J19" s="20">
-        <v>1</v>
-      </c>
-      <c r="K19" s="20">
-        <v>1</v>
-      </c>
-      <c r="L19" s="21">
+      <c r="B19" s="21">
+        <v>1</v>
+      </c>
+      <c r="C19" s="22">
+        <v>1</v>
+      </c>
+      <c r="D19" s="22">
+        <v>1</v>
+      </c>
+      <c r="E19" s="22">
+        <v>1</v>
+      </c>
+      <c r="F19" s="22">
+        <v>1</v>
+      </c>
+      <c r="G19" s="22">
+        <v>1</v>
+      </c>
+      <c r="H19" s="22">
+        <v>1</v>
+      </c>
+      <c r="I19" s="22">
+        <v>1</v>
+      </c>
+      <c r="J19" s="22">
+        <v>1</v>
+      </c>
+      <c r="K19" s="22">
+        <v>1</v>
+      </c>
+      <c r="L19" s="23">
         <v>10</v>
       </c>
       <c r="P19" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="Q19" s="19">
-        <v>1</v>
-      </c>
-      <c r="R19" s="20">
-        <v>1</v>
-      </c>
-      <c r="S19" s="20">
-        <v>1</v>
-      </c>
-      <c r="T19" s="20">
-        <v>1</v>
-      </c>
-      <c r="U19" s="20">
-        <v>1</v>
-      </c>
-      <c r="V19" s="20">
-        <v>1</v>
-      </c>
-      <c r="W19" s="20">
-        <v>1</v>
-      </c>
-      <c r="X19" s="20">
-        <v>1</v>
-      </c>
-      <c r="Y19" s="20">
-        <v>1</v>
-      </c>
-      <c r="Z19" s="20">
-        <v>1</v>
-      </c>
-      <c r="AA19" s="21">
+      <c r="Q19" s="21">
+        <v>1</v>
+      </c>
+      <c r="R19" s="22">
+        <v>1</v>
+      </c>
+      <c r="S19" s="22">
+        <v>1</v>
+      </c>
+      <c r="T19" s="22">
+        <v>1</v>
+      </c>
+      <c r="U19" s="22">
+        <v>1</v>
+      </c>
+      <c r="V19" s="22">
+        <v>1</v>
+      </c>
+      <c r="W19" s="22">
+        <v>1</v>
+      </c>
+      <c r="X19" s="22">
+        <v>1</v>
+      </c>
+      <c r="Y19" s="22">
+        <v>1</v>
+      </c>
+      <c r="Z19" s="22">
+        <v>1</v>
+      </c>
+      <c r="AA19" s="23">
         <v>10</v>
       </c>
     </row>
@@ -7392,73 +7392,73 @@
       <c r="A20" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="19">
-        <v>1</v>
-      </c>
-      <c r="C20" s="20">
-        <v>1</v>
-      </c>
-      <c r="D20" s="20">
-        <v>1</v>
-      </c>
-      <c r="E20" s="20">
-        <v>1</v>
-      </c>
-      <c r="F20" s="20">
-        <v>1</v>
-      </c>
-      <c r="G20" s="20">
-        <v>1</v>
-      </c>
-      <c r="H20" s="20">
-        <v>1</v>
-      </c>
-      <c r="I20" s="20">
-        <v>1</v>
-      </c>
-      <c r="J20" s="20">
-        <v>1</v>
-      </c>
-      <c r="K20" s="20">
-        <v>1</v>
-      </c>
-      <c r="L20" s="21">
+      <c r="B20" s="21">
+        <v>1</v>
+      </c>
+      <c r="C20" s="22">
+        <v>1</v>
+      </c>
+      <c r="D20" s="22">
+        <v>1</v>
+      </c>
+      <c r="E20" s="22">
+        <v>1</v>
+      </c>
+      <c r="F20" s="22">
+        <v>1</v>
+      </c>
+      <c r="G20" s="22">
+        <v>1</v>
+      </c>
+      <c r="H20" s="22">
+        <v>1</v>
+      </c>
+      <c r="I20" s="22">
+        <v>1</v>
+      </c>
+      <c r="J20" s="22">
+        <v>1</v>
+      </c>
+      <c r="K20" s="22">
+        <v>1</v>
+      </c>
+      <c r="L20" s="23">
         <v>10</v>
       </c>
       <c r="P20" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="Q20" s="19">
-        <v>1</v>
-      </c>
-      <c r="R20" s="20">
-        <v>1</v>
-      </c>
-      <c r="S20" s="20">
-        <v>1</v>
-      </c>
-      <c r="T20" s="20">
-        <v>1</v>
-      </c>
-      <c r="U20" s="20">
-        <v>1</v>
-      </c>
-      <c r="V20" s="20">
-        <v>1</v>
-      </c>
-      <c r="W20" s="20">
-        <v>1</v>
-      </c>
-      <c r="X20" s="20">
-        <v>1</v>
-      </c>
-      <c r="Y20" s="20">
-        <v>1</v>
-      </c>
-      <c r="Z20" s="20">
-        <v>1</v>
-      </c>
-      <c r="AA20" s="21">
+      <c r="Q20" s="21">
+        <v>1</v>
+      </c>
+      <c r="R20" s="22">
+        <v>1</v>
+      </c>
+      <c r="S20" s="22">
+        <v>1</v>
+      </c>
+      <c r="T20" s="22">
+        <v>1</v>
+      </c>
+      <c r="U20" s="22">
+        <v>1</v>
+      </c>
+      <c r="V20" s="22">
+        <v>1</v>
+      </c>
+      <c r="W20" s="22">
+        <v>1</v>
+      </c>
+      <c r="X20" s="22">
+        <v>1</v>
+      </c>
+      <c r="Y20" s="22">
+        <v>1</v>
+      </c>
+      <c r="Z20" s="22">
+        <v>1</v>
+      </c>
+      <c r="AA20" s="23">
         <v>10</v>
       </c>
     </row>
@@ -7466,73 +7466,73 @@
       <c r="A21" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="19">
-        <v>1</v>
-      </c>
-      <c r="C21" s="20">
-        <v>1</v>
-      </c>
-      <c r="D21" s="20">
-        <v>1</v>
-      </c>
-      <c r="E21" s="20">
-        <v>1</v>
-      </c>
-      <c r="F21" s="20">
-        <v>1</v>
-      </c>
-      <c r="G21" s="20">
-        <v>1</v>
-      </c>
-      <c r="H21" s="20">
-        <v>1</v>
-      </c>
-      <c r="I21" s="20">
-        <v>1</v>
-      </c>
-      <c r="J21" s="20">
-        <v>1</v>
-      </c>
-      <c r="K21" s="20">
-        <v>1</v>
-      </c>
-      <c r="L21" s="21">
+      <c r="B21" s="21">
+        <v>1</v>
+      </c>
+      <c r="C21" s="22">
+        <v>1</v>
+      </c>
+      <c r="D21" s="22">
+        <v>1</v>
+      </c>
+      <c r="E21" s="22">
+        <v>1</v>
+      </c>
+      <c r="F21" s="22">
+        <v>1</v>
+      </c>
+      <c r="G21" s="22">
+        <v>1</v>
+      </c>
+      <c r="H21" s="22">
+        <v>1</v>
+      </c>
+      <c r="I21" s="22">
+        <v>1</v>
+      </c>
+      <c r="J21" s="22">
+        <v>1</v>
+      </c>
+      <c r="K21" s="22">
+        <v>1</v>
+      </c>
+      <c r="L21" s="23">
         <v>10</v>
       </c>
       <c r="P21" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="Q21" s="19">
-        <v>1</v>
-      </c>
-      <c r="R21" s="20">
-        <v>1</v>
-      </c>
-      <c r="S21" s="20">
-        <v>1</v>
-      </c>
-      <c r="T21" s="20">
-        <v>1</v>
-      </c>
-      <c r="U21" s="20">
-        <v>1</v>
-      </c>
-      <c r="V21" s="20">
-        <v>1</v>
-      </c>
-      <c r="W21" s="20">
-        <v>1</v>
-      </c>
-      <c r="X21" s="20">
-        <v>1</v>
-      </c>
-      <c r="Y21" s="20">
-        <v>1</v>
-      </c>
-      <c r="Z21" s="20">
-        <v>1</v>
-      </c>
-      <c r="AA21" s="21">
+      <c r="Q21" s="21">
+        <v>1</v>
+      </c>
+      <c r="R21" s="22">
+        <v>1</v>
+      </c>
+      <c r="S21" s="22">
+        <v>1</v>
+      </c>
+      <c r="T21" s="22">
+        <v>1</v>
+      </c>
+      <c r="U21" s="22">
+        <v>1</v>
+      </c>
+      <c r="V21" s="22">
+        <v>1</v>
+      </c>
+      <c r="W21" s="22">
+        <v>1</v>
+      </c>
+      <c r="X21" s="22">
+        <v>1</v>
+      </c>
+      <c r="Y21" s="22">
+        <v>1</v>
+      </c>
+      <c r="Z21" s="22">
+        <v>1</v>
+      </c>
+      <c r="AA21" s="23">
         <v>10</v>
       </c>
     </row>
@@ -7540,73 +7540,73 @@
       <c r="A22" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="19">
-        <v>1</v>
-      </c>
-      <c r="C22" s="20">
-        <v>1</v>
-      </c>
-      <c r="D22" s="20">
-        <v>1</v>
-      </c>
-      <c r="E22" s="20">
-        <v>1</v>
-      </c>
-      <c r="F22" s="20">
-        <v>1</v>
-      </c>
-      <c r="G22" s="20">
-        <v>1</v>
-      </c>
-      <c r="H22" s="20">
-        <v>1</v>
-      </c>
-      <c r="I22" s="20">
-        <v>1</v>
-      </c>
-      <c r="J22" s="20">
-        <v>1</v>
-      </c>
-      <c r="K22" s="20">
-        <v>1</v>
-      </c>
-      <c r="L22" s="21">
+      <c r="B22" s="21">
+        <v>1</v>
+      </c>
+      <c r="C22" s="22">
+        <v>1</v>
+      </c>
+      <c r="D22" s="22">
+        <v>1</v>
+      </c>
+      <c r="E22" s="22">
+        <v>1</v>
+      </c>
+      <c r="F22" s="22">
+        <v>1</v>
+      </c>
+      <c r="G22" s="22">
+        <v>1</v>
+      </c>
+      <c r="H22" s="22">
+        <v>1</v>
+      </c>
+      <c r="I22" s="22">
+        <v>1</v>
+      </c>
+      <c r="J22" s="22">
+        <v>1</v>
+      </c>
+      <c r="K22" s="22">
+        <v>1</v>
+      </c>
+      <c r="L22" s="23">
         <v>10</v>
       </c>
       <c r="P22" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="Q22" s="19">
-        <v>1</v>
-      </c>
-      <c r="R22" s="20">
-        <v>1</v>
-      </c>
-      <c r="S22" s="20">
-        <v>1</v>
-      </c>
-      <c r="T22" s="20">
-        <v>1</v>
-      </c>
-      <c r="U22" s="20">
-        <v>1</v>
-      </c>
-      <c r="V22" s="20">
-        <v>1</v>
-      </c>
-      <c r="W22" s="20">
-        <v>1</v>
-      </c>
-      <c r="X22" s="20">
-        <v>1</v>
-      </c>
-      <c r="Y22" s="20">
-        <v>1</v>
-      </c>
-      <c r="Z22" s="20">
-        <v>1</v>
-      </c>
-      <c r="AA22" s="21">
+      <c r="Q22" s="21">
+        <v>1</v>
+      </c>
+      <c r="R22" s="22">
+        <v>1</v>
+      </c>
+      <c r="S22" s="22">
+        <v>1</v>
+      </c>
+      <c r="T22" s="22">
+        <v>1</v>
+      </c>
+      <c r="U22" s="22">
+        <v>1</v>
+      </c>
+      <c r="V22" s="22">
+        <v>1</v>
+      </c>
+      <c r="W22" s="22">
+        <v>1</v>
+      </c>
+      <c r="X22" s="22">
+        <v>1</v>
+      </c>
+      <c r="Y22" s="22">
+        <v>1</v>
+      </c>
+      <c r="Z22" s="22">
+        <v>1</v>
+      </c>
+      <c r="AA22" s="23">
         <v>10</v>
       </c>
     </row>
@@ -7614,73 +7614,73 @@
       <c r="A23" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="19">
-        <v>1</v>
-      </c>
-      <c r="C23" s="20">
-        <v>1</v>
-      </c>
-      <c r="D23" s="20">
-        <v>1</v>
-      </c>
-      <c r="E23" s="20">
-        <v>1</v>
-      </c>
-      <c r="F23" s="20">
-        <v>1</v>
-      </c>
-      <c r="G23" s="20">
-        <v>1</v>
-      </c>
-      <c r="H23" s="20">
-        <v>1</v>
-      </c>
-      <c r="I23" s="20">
-        <v>1</v>
-      </c>
-      <c r="J23" s="20">
-        <v>1</v>
-      </c>
-      <c r="K23" s="20">
-        <v>1</v>
-      </c>
-      <c r="L23" s="21">
+      <c r="B23" s="21">
+        <v>1</v>
+      </c>
+      <c r="C23" s="22">
+        <v>1</v>
+      </c>
+      <c r="D23" s="22">
+        <v>1</v>
+      </c>
+      <c r="E23" s="22">
+        <v>1</v>
+      </c>
+      <c r="F23" s="22">
+        <v>1</v>
+      </c>
+      <c r="G23" s="22">
+        <v>1</v>
+      </c>
+      <c r="H23" s="22">
+        <v>1</v>
+      </c>
+      <c r="I23" s="22">
+        <v>1</v>
+      </c>
+      <c r="J23" s="22">
+        <v>1</v>
+      </c>
+      <c r="K23" s="22">
+        <v>1</v>
+      </c>
+      <c r="L23" s="23">
         <v>10</v>
       </c>
       <c r="P23" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="Q23" s="19">
-        <v>1</v>
-      </c>
-      <c r="R23" s="20">
-        <v>1</v>
-      </c>
-      <c r="S23" s="20">
-        <v>1</v>
-      </c>
-      <c r="T23" s="20">
-        <v>1</v>
-      </c>
-      <c r="U23" s="20">
-        <v>1</v>
-      </c>
-      <c r="V23" s="20">
-        <v>1</v>
-      </c>
-      <c r="W23" s="20">
-        <v>1</v>
-      </c>
-      <c r="X23" s="20">
-        <v>1</v>
-      </c>
-      <c r="Y23" s="20">
-        <v>1</v>
-      </c>
-      <c r="Z23" s="20">
-        <v>1</v>
-      </c>
-      <c r="AA23" s="21">
+      <c r="Q23" s="21">
+        <v>1</v>
+      </c>
+      <c r="R23" s="22">
+        <v>1</v>
+      </c>
+      <c r="S23" s="22">
+        <v>1</v>
+      </c>
+      <c r="T23" s="22">
+        <v>1</v>
+      </c>
+      <c r="U23" s="22">
+        <v>1</v>
+      </c>
+      <c r="V23" s="22">
+        <v>1</v>
+      </c>
+      <c r="W23" s="22">
+        <v>1</v>
+      </c>
+      <c r="X23" s="22">
+        <v>1</v>
+      </c>
+      <c r="Y23" s="22">
+        <v>1</v>
+      </c>
+      <c r="Z23" s="22">
+        <v>1</v>
+      </c>
+      <c r="AA23" s="23">
         <v>10</v>
       </c>
     </row>
@@ -7688,73 +7688,73 @@
       <c r="A24" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="19">
-        <v>1</v>
-      </c>
-      <c r="C24" s="20">
-        <v>1</v>
-      </c>
-      <c r="D24" s="20">
-        <v>1</v>
-      </c>
-      <c r="E24" s="20">
-        <v>1</v>
-      </c>
-      <c r="F24" s="20">
-        <v>1</v>
-      </c>
-      <c r="G24" s="20">
-        <v>1</v>
-      </c>
-      <c r="H24" s="20">
-        <v>1</v>
-      </c>
-      <c r="I24" s="20">
-        <v>1</v>
-      </c>
-      <c r="J24" s="20">
-        <v>1</v>
-      </c>
-      <c r="K24" s="20">
-        <v>1</v>
-      </c>
-      <c r="L24" s="21">
+      <c r="B24" s="21">
+        <v>1</v>
+      </c>
+      <c r="C24" s="22">
+        <v>1</v>
+      </c>
+      <c r="D24" s="22">
+        <v>1</v>
+      </c>
+      <c r="E24" s="22">
+        <v>1</v>
+      </c>
+      <c r="F24" s="22">
+        <v>1</v>
+      </c>
+      <c r="G24" s="22">
+        <v>1</v>
+      </c>
+      <c r="H24" s="22">
+        <v>1</v>
+      </c>
+      <c r="I24" s="22">
+        <v>1</v>
+      </c>
+      <c r="J24" s="22">
+        <v>1</v>
+      </c>
+      <c r="K24" s="22">
+        <v>1</v>
+      </c>
+      <c r="L24" s="23">
         <v>10</v>
       </c>
       <c r="P24" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="Q24" s="19">
-        <v>1</v>
-      </c>
-      <c r="R24" s="20">
-        <v>1</v>
-      </c>
-      <c r="S24" s="20">
-        <v>1</v>
-      </c>
-      <c r="T24" s="20">
-        <v>1</v>
-      </c>
-      <c r="U24" s="20">
-        <v>1</v>
-      </c>
-      <c r="V24" s="20">
-        <v>1</v>
-      </c>
-      <c r="W24" s="20">
-        <v>1</v>
-      </c>
-      <c r="X24" s="20">
-        <v>1</v>
-      </c>
-      <c r="Y24" s="20">
-        <v>1</v>
-      </c>
-      <c r="Z24" s="20">
-        <v>1</v>
-      </c>
-      <c r="AA24" s="21">
+      <c r="Q24" s="21">
+        <v>1</v>
+      </c>
+      <c r="R24" s="22">
+        <v>1</v>
+      </c>
+      <c r="S24" s="22">
+        <v>1</v>
+      </c>
+      <c r="T24" s="22">
+        <v>1</v>
+      </c>
+      <c r="U24" s="22">
+        <v>1</v>
+      </c>
+      <c r="V24" s="22">
+        <v>1</v>
+      </c>
+      <c r="W24" s="22">
+        <v>1</v>
+      </c>
+      <c r="X24" s="22">
+        <v>1</v>
+      </c>
+      <c r="Y24" s="22">
+        <v>1</v>
+      </c>
+      <c r="Z24" s="22">
+        <v>1</v>
+      </c>
+      <c r="AA24" s="23">
         <v>10</v>
       </c>
     </row>
@@ -7762,73 +7762,73 @@
       <c r="A25" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="19">
-        <v>1</v>
-      </c>
-      <c r="C25" s="20">
-        <v>1</v>
-      </c>
-      <c r="D25" s="20">
-        <v>1</v>
-      </c>
-      <c r="E25" s="20">
-        <v>1</v>
-      </c>
-      <c r="F25" s="20">
-        <v>1</v>
-      </c>
-      <c r="G25" s="20">
-        <v>1</v>
-      </c>
-      <c r="H25" s="20">
-        <v>1</v>
-      </c>
-      <c r="I25" s="20">
-        <v>1</v>
-      </c>
-      <c r="J25" s="20">
-        <v>1</v>
-      </c>
-      <c r="K25" s="20">
-        <v>1</v>
-      </c>
-      <c r="L25" s="21">
+      <c r="B25" s="21">
+        <v>1</v>
+      </c>
+      <c r="C25" s="22">
+        <v>1</v>
+      </c>
+      <c r="D25" s="22">
+        <v>1</v>
+      </c>
+      <c r="E25" s="22">
+        <v>1</v>
+      </c>
+      <c r="F25" s="22">
+        <v>1</v>
+      </c>
+      <c r="G25" s="22">
+        <v>1</v>
+      </c>
+      <c r="H25" s="22">
+        <v>1</v>
+      </c>
+      <c r="I25" s="22">
+        <v>1</v>
+      </c>
+      <c r="J25" s="22">
+        <v>1</v>
+      </c>
+      <c r="K25" s="22">
+        <v>1</v>
+      </c>
+      <c r="L25" s="23">
         <v>10</v>
       </c>
       <c r="P25" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="Q25" s="19">
-        <v>1</v>
-      </c>
-      <c r="R25" s="20">
-        <v>1</v>
-      </c>
-      <c r="S25" s="20">
-        <v>1</v>
-      </c>
-      <c r="T25" s="20">
-        <v>1</v>
-      </c>
-      <c r="U25" s="20">
-        <v>1</v>
-      </c>
-      <c r="V25" s="20">
-        <v>1</v>
-      </c>
-      <c r="W25" s="20">
-        <v>1</v>
-      </c>
-      <c r="X25" s="20">
-        <v>1</v>
-      </c>
-      <c r="Y25" s="20">
-        <v>1</v>
-      </c>
-      <c r="Z25" s="20">
-        <v>1</v>
-      </c>
-      <c r="AA25" s="21">
+      <c r="Q25" s="21">
+        <v>1</v>
+      </c>
+      <c r="R25" s="22">
+        <v>1</v>
+      </c>
+      <c r="S25" s="22">
+        <v>1</v>
+      </c>
+      <c r="T25" s="22">
+        <v>1</v>
+      </c>
+      <c r="U25" s="22">
+        <v>1</v>
+      </c>
+      <c r="V25" s="22">
+        <v>1</v>
+      </c>
+      <c r="W25" s="22">
+        <v>1</v>
+      </c>
+      <c r="X25" s="22">
+        <v>1</v>
+      </c>
+      <c r="Y25" s="22">
+        <v>1</v>
+      </c>
+      <c r="Z25" s="22">
+        <v>1</v>
+      </c>
+      <c r="AA25" s="23">
         <v>10</v>
       </c>
     </row>
@@ -7836,73 +7836,73 @@
       <c r="A26" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="19">
-        <v>1</v>
-      </c>
-      <c r="C26" s="20">
-        <v>1</v>
-      </c>
-      <c r="D26" s="20">
-        <v>1</v>
-      </c>
-      <c r="E26" s="20">
-        <v>1</v>
-      </c>
-      <c r="F26" s="20">
-        <v>1</v>
-      </c>
-      <c r="G26" s="20">
-        <v>1</v>
-      </c>
-      <c r="H26" s="20">
-        <v>1</v>
-      </c>
-      <c r="I26" s="20">
-        <v>1</v>
-      </c>
-      <c r="J26" s="20">
-        <v>1</v>
-      </c>
-      <c r="K26" s="20">
-        <v>1</v>
-      </c>
-      <c r="L26" s="21">
+      <c r="B26" s="21">
+        <v>1</v>
+      </c>
+      <c r="C26" s="22">
+        <v>1</v>
+      </c>
+      <c r="D26" s="22">
+        <v>1</v>
+      </c>
+      <c r="E26" s="22">
+        <v>1</v>
+      </c>
+      <c r="F26" s="22">
+        <v>1</v>
+      </c>
+      <c r="G26" s="22">
+        <v>1</v>
+      </c>
+      <c r="H26" s="22">
+        <v>1</v>
+      </c>
+      <c r="I26" s="22">
+        <v>1</v>
+      </c>
+      <c r="J26" s="22">
+        <v>1</v>
+      </c>
+      <c r="K26" s="22">
+        <v>1</v>
+      </c>
+      <c r="L26" s="23">
         <v>10</v>
       </c>
       <c r="P26" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="Q26" s="19">
-        <v>1</v>
-      </c>
-      <c r="R26" s="20">
-        <v>1</v>
-      </c>
-      <c r="S26" s="20">
-        <v>1</v>
-      </c>
-      <c r="T26" s="20">
-        <v>1</v>
-      </c>
-      <c r="U26" s="20">
-        <v>1</v>
-      </c>
-      <c r="V26" s="20">
-        <v>1</v>
-      </c>
-      <c r="W26" s="20">
-        <v>1</v>
-      </c>
-      <c r="X26" s="20">
-        <v>1</v>
-      </c>
-      <c r="Y26" s="20">
-        <v>1</v>
-      </c>
-      <c r="Z26" s="20">
-        <v>1</v>
-      </c>
-      <c r="AA26" s="21">
+      <c r="Q26" s="21">
+        <v>1</v>
+      </c>
+      <c r="R26" s="22">
+        <v>1</v>
+      </c>
+      <c r="S26" s="22">
+        <v>1</v>
+      </c>
+      <c r="T26" s="22">
+        <v>1</v>
+      </c>
+      <c r="U26" s="22">
+        <v>1</v>
+      </c>
+      <c r="V26" s="22">
+        <v>1</v>
+      </c>
+      <c r="W26" s="22">
+        <v>1</v>
+      </c>
+      <c r="X26" s="22">
+        <v>1</v>
+      </c>
+      <c r="Y26" s="22">
+        <v>1</v>
+      </c>
+      <c r="Z26" s="22">
+        <v>1</v>
+      </c>
+      <c r="AA26" s="23">
         <v>10</v>
       </c>
     </row>
@@ -7910,73 +7910,73 @@
       <c r="A27" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="19">
-        <v>1</v>
-      </c>
-      <c r="C27" s="20">
-        <v>1</v>
-      </c>
-      <c r="D27" s="20">
-        <v>1</v>
-      </c>
-      <c r="E27" s="20">
-        <v>1</v>
-      </c>
-      <c r="F27" s="20">
-        <v>1</v>
-      </c>
-      <c r="G27" s="20">
-        <v>1</v>
-      </c>
-      <c r="H27" s="20">
-        <v>1</v>
-      </c>
-      <c r="I27" s="20">
-        <v>1</v>
-      </c>
-      <c r="J27" s="20">
-        <v>1</v>
-      </c>
-      <c r="K27" s="20">
-        <v>1</v>
-      </c>
-      <c r="L27" s="21">
+      <c r="B27" s="21">
+        <v>1</v>
+      </c>
+      <c r="C27" s="22">
+        <v>1</v>
+      </c>
+      <c r="D27" s="22">
+        <v>1</v>
+      </c>
+      <c r="E27" s="22">
+        <v>1</v>
+      </c>
+      <c r="F27" s="22">
+        <v>1</v>
+      </c>
+      <c r="G27" s="22">
+        <v>1</v>
+      </c>
+      <c r="H27" s="22">
+        <v>1</v>
+      </c>
+      <c r="I27" s="22">
+        <v>1</v>
+      </c>
+      <c r="J27" s="22">
+        <v>1</v>
+      </c>
+      <c r="K27" s="22">
+        <v>1</v>
+      </c>
+      <c r="L27" s="23">
         <v>10</v>
       </c>
       <c r="P27" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="Q27" s="19">
-        <v>1</v>
-      </c>
-      <c r="R27" s="20">
-        <v>1</v>
-      </c>
-      <c r="S27" s="20">
-        <v>1</v>
-      </c>
-      <c r="T27" s="20">
-        <v>1</v>
-      </c>
-      <c r="U27" s="20">
-        <v>1</v>
-      </c>
-      <c r="V27" s="20">
-        <v>1</v>
-      </c>
-      <c r="W27" s="20">
-        <v>1</v>
-      </c>
-      <c r="X27" s="20">
-        <v>1</v>
-      </c>
-      <c r="Y27" s="20">
-        <v>1</v>
-      </c>
-      <c r="Z27" s="20">
-        <v>1</v>
-      </c>
-      <c r="AA27" s="21">
+      <c r="Q27" s="21">
+        <v>1</v>
+      </c>
+      <c r="R27" s="22">
+        <v>1</v>
+      </c>
+      <c r="S27" s="22">
+        <v>1</v>
+      </c>
+      <c r="T27" s="22">
+        <v>1</v>
+      </c>
+      <c r="U27" s="22">
+        <v>1</v>
+      </c>
+      <c r="V27" s="22">
+        <v>1</v>
+      </c>
+      <c r="W27" s="22">
+        <v>1</v>
+      </c>
+      <c r="X27" s="22">
+        <v>1</v>
+      </c>
+      <c r="Y27" s="22">
+        <v>1</v>
+      </c>
+      <c r="Z27" s="22">
+        <v>1</v>
+      </c>
+      <c r="AA27" s="23">
         <v>10</v>
       </c>
     </row>
@@ -7984,73 +7984,73 @@
       <c r="A28" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="19">
-        <v>1</v>
-      </c>
-      <c r="C28" s="20">
-        <v>1</v>
-      </c>
-      <c r="D28" s="20">
-        <v>1</v>
-      </c>
-      <c r="E28" s="20">
-        <v>1</v>
-      </c>
-      <c r="F28" s="20">
-        <v>1</v>
-      </c>
-      <c r="G28" s="20">
-        <v>1</v>
-      </c>
-      <c r="H28" s="20">
-        <v>1</v>
-      </c>
-      <c r="I28" s="20">
-        <v>1</v>
-      </c>
-      <c r="J28" s="20">
-        <v>1</v>
-      </c>
-      <c r="K28" s="20">
-        <v>1</v>
-      </c>
-      <c r="L28" s="21">
+      <c r="B28" s="21">
+        <v>1</v>
+      </c>
+      <c r="C28" s="22">
+        <v>1</v>
+      </c>
+      <c r="D28" s="22">
+        <v>1</v>
+      </c>
+      <c r="E28" s="22">
+        <v>1</v>
+      </c>
+      <c r="F28" s="22">
+        <v>1</v>
+      </c>
+      <c r="G28" s="22">
+        <v>1</v>
+      </c>
+      <c r="H28" s="22">
+        <v>1</v>
+      </c>
+      <c r="I28" s="22">
+        <v>1</v>
+      </c>
+      <c r="J28" s="22">
+        <v>1</v>
+      </c>
+      <c r="K28" s="22">
+        <v>1</v>
+      </c>
+      <c r="L28" s="23">
         <v>10</v>
       </c>
       <c r="P28" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="Q28" s="19">
-        <v>1</v>
-      </c>
-      <c r="R28" s="20">
-        <v>1</v>
-      </c>
-      <c r="S28" s="20">
-        <v>1</v>
-      </c>
-      <c r="T28" s="20">
-        <v>1</v>
-      </c>
-      <c r="U28" s="20">
-        <v>1</v>
-      </c>
-      <c r="V28" s="20">
-        <v>1</v>
-      </c>
-      <c r="W28" s="20">
-        <v>1</v>
-      </c>
-      <c r="X28" s="20">
-        <v>1</v>
-      </c>
-      <c r="Y28" s="20">
-        <v>1</v>
-      </c>
-      <c r="Z28" s="20">
-        <v>1</v>
-      </c>
-      <c r="AA28" s="21">
+      <c r="Q28" s="21">
+        <v>1</v>
+      </c>
+      <c r="R28" s="22">
+        <v>1</v>
+      </c>
+      <c r="S28" s="22">
+        <v>1</v>
+      </c>
+      <c r="T28" s="22">
+        <v>1</v>
+      </c>
+      <c r="U28" s="22">
+        <v>1</v>
+      </c>
+      <c r="V28" s="22">
+        <v>1</v>
+      </c>
+      <c r="W28" s="22">
+        <v>1</v>
+      </c>
+      <c r="X28" s="22">
+        <v>1</v>
+      </c>
+      <c r="Y28" s="22">
+        <v>1</v>
+      </c>
+      <c r="Z28" s="22">
+        <v>1</v>
+      </c>
+      <c r="AA28" s="23">
         <v>10</v>
       </c>
     </row>
@@ -8058,73 +8058,73 @@
       <c r="A29" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="19">
-        <v>1</v>
-      </c>
-      <c r="C29" s="20">
-        <v>1</v>
-      </c>
-      <c r="D29" s="20">
-        <v>1</v>
-      </c>
-      <c r="E29" s="20">
-        <v>1</v>
-      </c>
-      <c r="F29" s="20">
-        <v>1</v>
-      </c>
-      <c r="G29" s="20">
-        <v>1</v>
-      </c>
-      <c r="H29" s="20">
-        <v>1</v>
-      </c>
-      <c r="I29" s="20">
-        <v>1</v>
-      </c>
-      <c r="J29" s="20">
-        <v>1</v>
-      </c>
-      <c r="K29" s="20">
-        <v>1</v>
-      </c>
-      <c r="L29" s="21">
+      <c r="B29" s="21">
+        <v>1</v>
+      </c>
+      <c r="C29" s="22">
+        <v>1</v>
+      </c>
+      <c r="D29" s="22">
+        <v>1</v>
+      </c>
+      <c r="E29" s="22">
+        <v>1</v>
+      </c>
+      <c r="F29" s="22">
+        <v>1</v>
+      </c>
+      <c r="G29" s="22">
+        <v>1</v>
+      </c>
+      <c r="H29" s="22">
+        <v>1</v>
+      </c>
+      <c r="I29" s="22">
+        <v>1</v>
+      </c>
+      <c r="J29" s="22">
+        <v>1</v>
+      </c>
+      <c r="K29" s="22">
+        <v>1</v>
+      </c>
+      <c r="L29" s="23">
         <v>10</v>
       </c>
       <c r="P29" s="9" t="s">
         <v>394</v>
       </c>
-      <c r="Q29" s="22">
+      <c r="Q29" s="24">
         <v>24</v>
       </c>
-      <c r="R29" s="23">
+      <c r="R29" s="25">
         <v>24</v>
       </c>
-      <c r="S29" s="23">
+      <c r="S29" s="25">
         <v>24</v>
       </c>
-      <c r="T29" s="23">
+      <c r="T29" s="25">
         <v>24</v>
       </c>
-      <c r="U29" s="23">
+      <c r="U29" s="25">
         <v>24</v>
       </c>
-      <c r="V29" s="23">
+      <c r="V29" s="25">
         <v>24</v>
       </c>
-      <c r="W29" s="23">
+      <c r="W29" s="25">
         <v>24</v>
       </c>
-      <c r="X29" s="23">
+      <c r="X29" s="25">
         <v>24</v>
       </c>
-      <c r="Y29" s="23">
+      <c r="Y29" s="25">
         <v>24</v>
       </c>
-      <c r="Z29" s="23">
+      <c r="Z29" s="25">
         <v>24</v>
       </c>
-      <c r="AA29" s="24">
+      <c r="AA29" s="26">
         <v>240</v>
       </c>
     </row>
@@ -8132,37 +8132,37 @@
       <c r="A30" s="9" t="s">
         <v>394</v>
       </c>
-      <c r="B30" s="22">
+      <c r="B30" s="24">
         <v>25</v>
       </c>
-      <c r="C30" s="23">
+      <c r="C30" s="25">
         <v>25</v>
       </c>
-      <c r="D30" s="23">
+      <c r="D30" s="25">
         <v>25</v>
       </c>
-      <c r="E30" s="23">
+      <c r="E30" s="25">
         <v>25</v>
       </c>
-      <c r="F30" s="23">
+      <c r="F30" s="25">
         <v>25</v>
       </c>
-      <c r="G30" s="23">
+      <c r="G30" s="25">
         <v>25</v>
       </c>
-      <c r="H30" s="23">
+      <c r="H30" s="25">
         <v>25</v>
       </c>
-      <c r="I30" s="23">
+      <c r="I30" s="25">
         <v>25</v>
       </c>
-      <c r="J30" s="23">
+      <c r="J30" s="25">
         <v>25</v>
       </c>
-      <c r="K30" s="23">
+      <c r="K30" s="25">
         <v>25</v>
       </c>
-      <c r="L30" s="24">
+      <c r="L30" s="26">
         <v>250</v>
       </c>
     </row>
@@ -9146,7 +9146,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F904477C-6323-401B-B08E-7A01032FDF06}">
   <dimension ref="A3:M32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
@@ -10269,7 +10269,7 @@
     </row>
   </sheetData>
   <conditionalFormatting pivot="1" sqref="B5:K30">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10281,7 +10281,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E1007"/>
   <sheetViews>
-    <sheetView topLeftCell="A243" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A251" workbookViewId="0">
       <selection activeCell="D267" sqref="D267"/>
     </sheetView>
   </sheetViews>
@@ -10294,7 +10294,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="17" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -14483,7 +14483,7 @@
     </row>
     <row r="263" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="264" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C264" s="26" t="s">
+      <c r="C264" s="17" t="s">
         <v>399</v>
       </c>
       <c r="D264">
@@ -14492,7 +14492,7 @@
       </c>
     </row>
     <row r="265" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C265" s="26" t="s">
+      <c r="C265" s="17" t="s">
         <v>400</v>
       </c>
       <c r="D265">
@@ -14501,16 +14501,16 @@
       </c>
     </row>
     <row r="266" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C266" s="26" t="s">
+      <c r="C266" s="17" t="s">
         <v>401</v>
       </c>
-      <c r="D266" s="25">
+      <c r="D266" s="16">
         <f>AVERAGE(D2:D261)*1000</f>
         <v>744484.61538461538</v>
       </c>
     </row>
     <row r="267" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C267" s="26" t="s">
+      <c r="C267" s="17" t="s">
         <v>402</v>
       </c>
       <c r="D267">
@@ -14519,7 +14519,7 @@
       </c>
     </row>
     <row r="268" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C268" s="26" t="s">
+      <c r="C268" s="17" t="s">
         <v>403</v>
       </c>
     </row>
@@ -15278,8 +15278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B52D43FB-93FF-4FA5-901D-F9DEF2AE9E5C}">
   <dimension ref="A1:A181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="A182" sqref="A182"/>
+    <sheetView topLeftCell="A161" workbookViewId="0">
+      <selection activeCell="A181" sqref="A181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>